<commit_message>
Practiced Logistic regression model.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,12 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="4">
   <si>
     <t>age</t>
   </si>
   <si>
-    <t>eligibility</t>
+    <t>inssurance</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>yes</t>
   </si>
 </sst>
 </file>
@@ -377,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -396,10 +402,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>33</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -407,10 +413,10 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -418,10 +424,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>48</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -429,10 +435,10 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>55</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -440,10 +446,10 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>51</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -451,10 +457,10 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>21</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -462,10 +468,10 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>36</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -473,10 +479,10 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>43</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -484,10 +490,10 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>60</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -497,8 +503,8 @@
       <c r="B11">
         <v>34</v>
       </c>
-      <c r="C11">
-        <v>0</v>
+      <c r="C11" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -506,10 +512,10 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>40</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -517,10 +523,10 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>55</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -528,10 +534,10 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>36</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -539,10 +545,10 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>26</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
+        <v>25</v>
+      </c>
+      <c r="C15" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -550,10 +556,10 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>27</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -561,10 +567,10 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>32</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -572,10 +578,10 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>54</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
+        <v>25</v>
+      </c>
+      <c r="C18" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -583,10 +589,10 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>49</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -594,21 +600,10 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>57</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21">
-        <v>44</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>